<commit_message>
burn down chart updated again
</commit_message>
<xml_diff>
--- a/Planning/Burndown Chart.xlsx
+++ b/Planning/Burndown Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moksh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3364E633-3ACD-4091-B817-028CD7B65986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{936D3857-3455-4D49-BA21-27076E12C2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73D86F60-A37F-4B90-8D7A-D0CD68C7E12A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Calendar Days </t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Actual</t>
+  </si>
+  <si>
+    <t>Velocity = 5 story points/sprint</t>
   </si>
 </sst>
 </file>
@@ -325,13 +328,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
@@ -346,73 +349,73 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="22">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="23">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="24">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="25">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="26">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="29">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0</c:v>
@@ -580,25 +583,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1715,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9C9C93-3B88-42B6-AAFE-471811ED177B}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="121" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="121" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1737,10 +1752,10 @@
         <v>45713</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1748,10 +1763,10 @@
         <v>45714</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1759,10 +1774,10 @@
         <v>45715</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1773,7 +1788,7 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1784,7 +1799,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1795,7 +1810,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1806,7 +1821,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1814,7 +1829,10 @@
         <v>45720</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1822,7 +1840,10 @@
         <v>45721</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1830,7 +1851,10 @@
         <v>45722</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1838,7 +1862,10 @@
         <v>45723</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1846,7 +1873,7 @@
         <v>45724</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1854,7 +1881,7 @@
         <v>45725</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1862,7 +1889,7 @@
         <v>45726</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1870,7 +1897,7 @@
         <v>45727</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1878,7 +1905,7 @@
         <v>45728</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1886,7 +1913,7 @@
         <v>45729</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1894,7 +1921,7 @@
         <v>45730</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1902,7 +1929,7 @@
         <v>45731</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1910,7 +1937,7 @@
         <v>45732</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1918,7 +1945,7 @@
         <v>45733</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1926,7 +1953,7 @@
         <v>45734</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -1934,7 +1961,7 @@
         <v>45735</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -1942,7 +1969,7 @@
         <v>45736</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -1950,7 +1977,7 @@
         <v>45737</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1958,7 +1985,7 @@
         <v>45738</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1966,7 +1993,7 @@
         <v>45739</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1974,7 +2001,7 @@
         <v>45740</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1982,7 +2009,7 @@
         <v>45741</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -1990,7 +2017,7 @@
         <v>45742</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -2016,7 +2043,9 @@
       <c r="A35" s="1"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>

</xml_diff>